<commit_message>
Fix shifting formulas (during insert/delete/sort) Fix sorting of differently typed values Some performance improvements (structs can be slow!)
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/ShiftingFormulas.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/ShiftingFormulas.xlsx
@@ -10,8 +10,8 @@
     <x:sheet name="WS2" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="WorksheetB4C4" localSheetId="0">'Shifting Formulas'!$C$5:$D$5</x:definedName>
-    <x:definedName name="WorkbookB4C4">'Shifting Formulas'!$C$5:$D$5</x:definedName>
+    <x:definedName name="WorksheetB4C4" localSheetId="0">'Shifting Formulas'!$C$4:$D$4</x:definedName>
+    <x:definedName name="WorkbookB4C4">'Shifting Formulas'!$C$4:$D$4</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
@@ -394,7 +394,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G5"/>
+  <x:dimension ref="A1:G4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -403,43 +403,43 @@
     <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
+    <x:row r="2" spans="1:7">
+      <x:c r="C2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E2" s="0">
+        <x:f>SUM(C2:D2)</x:f>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="G2" s="0">
+        <x:f>Average(C2:D3)</x:f>
+      </x:c>
+    </x:row>
     <x:row r="3" spans="1:7">
       <x:c r="C3" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="E3" s="0">
         <x:f>SUM(C3:D3)</x:f>
       </x:c>
-      <x:c r="F3" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="G3" s="0">
-        <x:f>Average(C3:D4)</x:f>
-      </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
-      <x:c r="C4" s="0" t="n">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="E4" s="0">
-        <x:f>SUM(C4:D4)</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="B5" s="1" t="s">
+      <x:c r="B4" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C5" s="0">
-        <x:f>Sum(C3:C4)</x:f>
-      </x:c>
-      <x:c r="D5" s="0">
-        <x:f>Sum(D3:D4)</x:f>
+      <x:c r="C4" s="0">
+        <x:f>Sum(C2:C3)</x:f>
+      </x:c>
+      <x:c r="D4" s="0">
+        <x:f>Sum(D2:D3)</x:f>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -464,7 +464,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:2">
       <x:c r="A1" s="0">
-        <x:f>'Shifting Formulas'!C3</x:f>
+        <x:f>'Shifting Formulas'!#REF!</x:f>
       </x:c>
       <x:c r="B1" s="0" t="n">
         <x:v>5</x:v>
@@ -472,42 +472,42 @@
     </x:row>
     <x:row r="2" spans="1:2">
       <x:c r="A2" s="0">
-        <x:f>Average('Shifting Formulas'!$C$3:$D$4)</x:f>
+        <x:f>Average('Shifting Formulas'!$C$2:$D$3)</x:f>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:2">
       <x:c r="A3" s="0">
-        <x:f>Average('Shifting Formulas'!$C$3:$D4)</x:f>
+        <x:f>Average('Shifting Formulas'!$C$2:$D3)</x:f>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:2">
       <x:c r="A4" s="0">
-        <x:f>Average('Shifting Formulas'!$C$3:D4)</x:f>
+        <x:f>Average('Shifting Formulas'!$C$2:D3)</x:f>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:2">
       <x:c r="A5" s="0">
-        <x:f>Average('Shifting Formulas'!$C3:D4)</x:f>
+        <x:f>Average('Shifting Formulas'!$C2:D3)</x:f>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
       <x:c r="A6" s="0">
-        <x:f>Average('Shifting Formulas'!C3:D4)</x:f>
+        <x:f>Average('Shifting Formulas'!C2:D3)</x:f>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
       <x:c r="A7" s="0">
-        <x:f>Average('Shifting Formulas'!C3:D$4)</x:f>
+        <x:f>Average('Shifting Formulas'!C2:D$3)</x:f>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
       <x:c r="A8" s="0">
-        <x:f>Average('Shifting Formulas'!C3:$D$4)</x:f>
+        <x:f>Average('Shifting Formulas'!C2:$D$3)</x:f>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:2">
       <x:c r="A9" s="0">
-        <x:f>Average('Shifting Formulas'!C$3:$D$4)</x:f>
+        <x:f>Average('Shifting Formulas'!C$2:$D$3)</x:f>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>